<commit_message>
getting students time interval correctly
</commit_message>
<xml_diff>
--- a/stufreeEdited.xlsx
+++ b/stufreeEdited.xlsx
@@ -539,7 +539,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>['4']</t>
+          <t>['4', '4:30']</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>['2', '2:30', '3', '3:30', '4']</t>
+          <t>['2', '2:30', '3', '3:30', '4', '4:30']</t>
         </is>
       </c>
     </row>
@@ -583,7 +583,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>['12:30', '1', '1:30'] and  ['3', '3:30', '4']</t>
+          <t xml:space="preserve">['12:30', '1', '1:30'] and  ['3', '3:30', '4', '4:30']  </t>
         </is>
       </c>
     </row>
@@ -649,7 +649,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>['10', '10:30', '11', '11:30', '12', '12:30'] and  ['3', '3:30', '4']</t>
+          <t xml:space="preserve">['10', '10:30', '11', '11:30', '12', '12:30'] and  ['3', '3:30', '4', '4:30']  </t>
         </is>
       </c>
     </row>
@@ -671,7 +671,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>['3', '3:30', '4']</t>
+          <t>['3', '3:30', '4', '4:30']</t>
         </is>
       </c>
     </row>
@@ -715,7 +715,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>['1', '1:30', '2', '2:30', '3', '3:30', '4']</t>
+          <t>['1', '1:30', '2', '2:30', '3', '3:30', '4', '4:30']</t>
         </is>
       </c>
     </row>
@@ -781,7 +781,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>['11', '11:30', '12', '12:30', '1', '1:30', '2', '2:30', '3', '3:30', '4']</t>
+          <t>['11', '11:30', '12', '12:30', '1', '1:30', '2', '2:30', '3', '3:30', '4', '4:30']</t>
         </is>
       </c>
     </row>
@@ -803,7 +803,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>['10', '10:30', '11', '11:30', '12', '12:30', '1', '1:30', '2', '2:30', '3', '3:30', '4']</t>
+          <t>['10', '10:30', '11', '11:30', '12', '12:30', '1', '1:30', '2', '2:30', '3', '3:30', '4', '4:30']</t>
         </is>
       </c>
     </row>
@@ -847,7 +847,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>['10', '10:30', '11', '11:30', '12', '12:30', '1', '1:30', '2', '2:30', '3', '3:30', '4']</t>
+          <t>['10', '10:30', '11', '11:30', '12', '12:30', '1', '1:30', '2', '2:30', '3', '3:30', '4', '4:30']</t>
         </is>
       </c>
     </row>
@@ -869,7 +869,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>['11', '11:30', '12', '12:30', '1', '1:30'] and  ['4']</t>
+          <t xml:space="preserve">['11', '11:30', '12', '12:30', '1', '1:30'] and  ['4', '4:30']  </t>
         </is>
       </c>
     </row>
@@ -891,7 +891,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>['1', '1:30', '2', '2:30', '3', '3:30', '4']</t>
+          <t>['1', '1:30', '2', '2:30', '3', '3:30', '4', '4:30']</t>
         </is>
       </c>
     </row>
@@ -935,7 +935,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>['10', '10:30', '11', '11:30', '12', '12:30', '1', '1:30', '2', '2:30', '3', '3:30', '4']</t>
+          <t>['10', '10:30', '11', '11:30', '12', '12:30', '1', '1:30', '2', '2:30', '3', '3:30', '4', '4:30']</t>
         </is>
       </c>
     </row>
@@ -957,7 +957,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>['10', '10:30', '11', '11:30', '12', '12:30', '1', '1:30', '2', '2:30', '3', '3:30', '4']</t>
+          <t>['10', '10:30', '11', '11:30', '12', '12:30', '1', '1:30', '2', '2:30', '3', '3:30', '4', '4:30']</t>
         </is>
       </c>
     </row>
@@ -979,7 +979,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>['4']</t>
+          <t>['4', '4:30']</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>['12', '12:30', '1', '1:30', '2', '2:30', '3', '3:30', '4']</t>
+          <t>['12', '12:30', '1', '1:30', '2', '2:30', '3', '3:30', '4', '4:30']</t>
         </is>
       </c>
     </row>
@@ -1023,7 +1023,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>['11', '11:30', '12', '12:30', '1', '1:30'] and  ['4']</t>
+          <t xml:space="preserve">['11', '11:30', '12', '12:30', '1', '1:30'] and  ['4', '4:30']  </t>
         </is>
       </c>
     </row>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>['10', '10:30'] and  ['1', '1:30', '2', '2:30', '3', '3:30', '4']</t>
+          <t xml:space="preserve">['10', '10:30'] and  ['1', '1:30', '2', '2:30', '3', '3:30', '4', '4:30']  </t>
         </is>
       </c>
     </row>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>['10', '10:30', '11', '11:30', '12', '12:30', '1', '1:30', '2', '2:30', '3', '3:30', '4']</t>
+          <t>['10', '10:30', '11', '11:30', '12', '12:30', '1', '1:30', '2', '2:30', '3', '3:30', '4', '4:30']</t>
         </is>
       </c>
     </row>
@@ -1111,7 +1111,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>['10', '10:30', '11', '11:30', '12', '12:30', '1', '1:30', '2'] and  ['4']</t>
+          <t xml:space="preserve">['10', '10:30', '11', '11:30', '12', '12:30', '1', '1:30', '2'] and  ['4', '4:30']  </t>
         </is>
       </c>
     </row>
@@ -1133,7 +1133,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>['1', '1:30', '2', '2:30', '3', '3:30', '4']</t>
+          <t>['1', '1:30', '2', '2:30', '3', '3:30', '4', '4:30']</t>
         </is>
       </c>
     </row>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>['10', '10:30', '11', '11:30', '12', '12:30', '1', '1:30', '2', '2:30', '3', '3:30', '4']</t>
+          <t>['10', '10:30', '11', '11:30', '12', '12:30', '1', '1:30', '2', '2:30', '3', '3:30', '4', '4:30']</t>
         </is>
       </c>
     </row>
@@ -1177,7 +1177,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>['1', '1:30', '2', '2:30', '3', '3:30', '4']</t>
+          <t>['1', '1:30', '2', '2:30', '3', '3:30', '4', '4:30']</t>
         </is>
       </c>
     </row>
@@ -1199,7 +1199,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>['1', '1:30', '2', '2:30', '3', '3:30', '4']</t>
+          <t>['1', '1:30', '2', '2:30', '3', '3:30', '4', '4:30']</t>
         </is>
       </c>
     </row>
@@ -1221,7 +1221,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>['10', '10:30', '11', '11:30', '12', '12:30', '1', '1:30', '2', '2:30', '3', '3:30', '4']</t>
+          <t>['10', '10:30', '11', '11:30', '12', '12:30', '1', '1:30', '2', '2:30', '3', '3:30', '4', '4:30']</t>
         </is>
       </c>
     </row>
@@ -1243,7 +1243,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>['1:30', '2', '2:30', '3', '3:30', '4']</t>
+          <t>['1:30', '2', '2:30', '3', '3:30', '4', '4:30']</t>
         </is>
       </c>
     </row>
@@ -1265,7 +1265,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>['2', '2:30', '3', '3:30', '4']</t>
+          <t>['2', '2:30', '3', '3:30', '4', '4:30']</t>
         </is>
       </c>
     </row>
@@ -1287,7 +1287,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>['12', '12:30', '1', '1:30', '2', '2:30', '3', '3:30', '4']</t>
+          <t>['12', '12:30', '1', '1:30', '2', '2:30', '3', '3:30', '4', '4:30']</t>
         </is>
       </c>
     </row>
@@ -1309,7 +1309,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>['10', '10:30', '11', '11:30'] and  ['3', '3:30', '4']</t>
+          <t xml:space="preserve">['10', '10:30', '11', '11:30'] and  ['3', '3:30', '4', '4:30']  </t>
         </is>
       </c>
     </row>
@@ -1331,7 +1331,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>['3:30', '4']</t>
+          <t>['3:30', '4', '4:30']</t>
         </is>
       </c>
     </row>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>['3', '3:30', '4']</t>
+          <t>['3', '3:30', '4', '4:30']</t>
         </is>
       </c>
     </row>
@@ -1375,7 +1375,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>['1', '1:30', '2', '2:30', '3', '3:30', '4']</t>
+          <t>['1', '1:30', '2', '2:30', '3', '3:30', '4', '4:30']</t>
         </is>
       </c>
     </row>
@@ -1397,7 +1397,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>['12', '12:30', '1', '1:30', '2', '2:30', '3', '3:30', '4']</t>
+          <t>['12', '12:30', '1', '1:30', '2', '2:30', '3', '3:30', '4', '4:30']</t>
         </is>
       </c>
     </row>
@@ -1419,7 +1419,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>['1', '1:30', '2', '2:30', '3', '3:30', '4']</t>
+          <t>['1', '1:30', '2', '2:30', '3', '3:30', '4', '4:30']</t>
         </is>
       </c>
     </row>

</xml_diff>